<commit_message>
feat: fix some missing data, add combine script and final.csv
</commit_message>
<xml_diff>
--- a/bengkulu/bengkulu-mei.xlsx
+++ b/bengkulu/bengkulu-mei.xlsx
@@ -15,36 +15,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>ID WMO</t>
   </si>
   <si>
-    <t>:  96255</t>
+    <t>:  96253</t>
   </si>
   <si>
     <t>NAMA STASIUN</t>
   </si>
   <si>
-    <t>:  Stasiun Klimatologi Bengkulu</t>
+    <t>:  Stasiun Meteorologi Fatmawati Soekarno</t>
   </si>
   <si>
     <t>LINTANG</t>
   </si>
   <si>
-    <t>:  -3.86520</t>
+    <t>:  -3.85820</t>
   </si>
   <si>
     <t>BUJUR</t>
   </si>
   <si>
-    <t>:  102.31190</t>
+    <t>:  102.33670</t>
   </si>
   <si>
     <t>ELEVASI</t>
   </si>
   <si>
-    <t>:  12 Meter</t>
+    <t>:  24 Meter</t>
   </si>
   <si>
     <t>TANGGAL</t>
@@ -83,85 +83,112 @@
     <t>01-05-2025</t>
   </si>
   <si>
-    <t>SW</t>
+    <t>E</t>
   </si>
   <si>
     <t>02-05-2025</t>
   </si>
   <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>03-05-2025</t>
+  </si>
+  <si>
+    <t>04-05-2025</t>
+  </si>
+  <si>
+    <t>05-05-2025</t>
+  </si>
+  <si>
+    <t>06-05-2025</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>07-05-2025</t>
+  </si>
+  <si>
+    <t>08-05-2025</t>
+  </si>
+  <si>
     <t>W</t>
   </si>
   <si>
-    <t>03-05-2025</t>
-  </si>
-  <si>
-    <t>04-05-2025</t>
-  </si>
-  <si>
-    <t>05-05-2025</t>
-  </si>
-  <si>
-    <t>06-05-2025</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>07-05-2025</t>
+    <t>09-05-2025</t>
+  </si>
+  <si>
+    <t>10-05-2025</t>
+  </si>
+  <si>
+    <t>11-05-2025</t>
+  </si>
+  <si>
+    <t>12-05-2025</t>
+  </si>
+  <si>
+    <t>13-05-2025</t>
+  </si>
+  <si>
+    <t>14-05-2025</t>
+  </si>
+  <si>
+    <t>15-05-2025</t>
+  </si>
+  <si>
+    <t>16-05-2025</t>
+  </si>
+  <si>
+    <t>17-05-2025</t>
+  </si>
+  <si>
+    <t>18-05-2025</t>
+  </si>
+  <si>
+    <t>19-05-2025</t>
+  </si>
+  <si>
+    <t>20-05-2025</t>
+  </si>
+  <si>
+    <t>21-05-2025</t>
+  </si>
+  <si>
+    <t>22-05-2025</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>23-05-2025</t>
+  </si>
+  <si>
+    <t>24-05-2025</t>
+  </si>
+  <si>
+    <t>25-05-2025</t>
+  </si>
+  <si>
+    <t>26-05-2025</t>
+  </si>
+  <si>
+    <t>27-05-2025</t>
+  </si>
+  <si>
+    <t>28-05-2025</t>
+  </si>
+  <si>
+    <t>29-05-2025</t>
+  </si>
+  <si>
+    <t>30-05-2025</t>
   </si>
   <si>
     <t>SE</t>
   </si>
   <si>
-    <t>08-05-2025</t>
-  </si>
-  <si>
-    <t>09-05-2025</t>
-  </si>
-  <si>
-    <t>10-05-2025</t>
-  </si>
-  <si>
-    <t>11-05-2025</t>
-  </si>
-  <si>
-    <t>12-05-2025</t>
-  </si>
-  <si>
-    <t>13-05-2025</t>
-  </si>
-  <si>
-    <t>14-05-2025</t>
-  </si>
-  <si>
-    <t>15-05-2025</t>
-  </si>
-  <si>
-    <t>16-05-2025</t>
-  </si>
-  <si>
-    <t>17-05-2025</t>
-  </si>
-  <si>
-    <t>18-05-2025</t>
-  </si>
-  <si>
-    <t>19-05-2025</t>
-  </si>
-  <si>
-    <t>20-05-2025</t>
-  </si>
-  <si>
-    <t>21-05-2025</t>
-  </si>
-  <si>
-    <t>22-05-2025</t>
-  </si>
-  <si>
-    <t>23-05-2025</t>
-  </si>
-  <si>
-    <t>24-05-2025</t>
+    <t>31-05-2025</t>
   </si>
   <si>
     <t>KETERANGAN:</t>
@@ -616,10 +643,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A33" sqref="A33:K33"/>
+      <selection activeCell="A40" sqref="A40:K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -709,28 +736,28 @@
         <v>21</v>
       </c>
       <c r="B9" s="2">
-        <v>24.8</v>
+        <v>24.6</v>
       </c>
       <c r="C9" s="2">
-        <v>32.5</v>
+        <v>32.1</v>
       </c>
       <c r="D9" s="2">
-        <v>27.7</v>
+        <v>27.5</v>
       </c>
       <c r="E9" s="2">
-        <v>87.0</v>
+        <v>86.0</v>
       </c>
       <c r="F9" s="2">
         <v>8888.0</v>
       </c>
       <c r="G9" s="2">
-        <v>5.4</v>
+        <v>3.7</v>
       </c>
       <c r="H9" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I9" s="2">
-        <v>250</v>
+        <v>230</v>
       </c>
       <c r="J9" s="2">
         <v>2.0</v>
@@ -744,28 +771,28 @@
         <v>23</v>
       </c>
       <c r="B10" s="2">
-        <v>25.2</v>
+        <v>25.0</v>
       </c>
       <c r="C10" s="2">
-        <v>31.6</v>
+        <v>32.2</v>
       </c>
       <c r="D10" s="2">
-        <v>27.6</v>
+        <v>27.9</v>
       </c>
       <c r="E10" s="2">
-        <v>89.0</v>
+        <v>84.0</v>
       </c>
       <c r="F10" s="2">
-        <v>8.5</v>
+        <v>3.8</v>
       </c>
       <c r="G10" s="2">
-        <v>8.0</v>
+        <v>7.7</v>
       </c>
       <c r="H10" s="2">
         <v>4.0</v>
       </c>
       <c r="I10" s="2">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="J10" s="2">
         <v>2.0</v>
@@ -779,34 +806,34 @@
         <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>24.8</v>
+        <v>24.6</v>
       </c>
       <c r="C11" s="2">
-        <v>32.5</v>
+        <v>32.9</v>
       </c>
       <c r="D11" s="2">
         <v>27.8</v>
       </c>
       <c r="E11" s="2">
-        <v>86.0</v>
+        <v>81.0</v>
       </c>
       <c r="F11" s="2">
-        <v>0.4</v>
+        <v>4.2</v>
       </c>
       <c r="G11" s="2">
-        <v>6.3</v>
+        <v>5.8</v>
       </c>
       <c r="H11" s="2">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="I11" s="2">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="J11" s="2">
         <v>2.0</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -814,16 +841,16 @@
         <v>26</v>
       </c>
       <c r="B12" s="2">
-        <v>24.8</v>
+        <v>24.7</v>
       </c>
       <c r="C12" s="2">
-        <v>32.1</v>
+        <v>33.2</v>
       </c>
       <c r="D12" s="2">
-        <v>27.8</v>
+        <v>28.0</v>
       </c>
       <c r="E12" s="2">
-        <v>86.0</v>
+        <v>82.0</v>
       </c>
       <c r="F12" s="2">
         <v>0.0</v>
@@ -832,16 +859,16 @@
         <v>8.0</v>
       </c>
       <c r="H12" s="2">
-        <v>4.0</v>
+        <v>8.0</v>
       </c>
       <c r="I12" s="2">
-        <v>280</v>
+        <v>70</v>
       </c>
       <c r="J12" s="2">
         <v>2.0</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -849,34 +876,34 @@
         <v>27</v>
       </c>
       <c r="B13" s="2">
-        <v>24.4</v>
+        <v>24.3</v>
       </c>
       <c r="C13" s="2">
-        <v>31.9</v>
+        <v>32.6</v>
       </c>
       <c r="D13" s="2">
-        <v>27.6</v>
+        <v>27.7</v>
       </c>
       <c r="E13" s="2">
-        <v>84.0</v>
+        <v>81.0</v>
       </c>
       <c r="F13" s="2">
         <v>0.0</v>
       </c>
       <c r="G13" s="2">
-        <v>6.6</v>
+        <v>4.9</v>
       </c>
       <c r="H13" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I13" s="2">
-        <v>270</v>
+        <v>250</v>
       </c>
       <c r="J13" s="2">
         <v>2.0</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -884,16 +911,16 @@
         <v>28</v>
       </c>
       <c r="B14" s="2">
-        <v>24.7</v>
+        <v>25.0</v>
       </c>
       <c r="C14" s="2">
-        <v>32.9</v>
+        <v>33.2</v>
       </c>
       <c r="D14" s="2">
-        <v>28.6</v>
+        <v>28.9</v>
       </c>
       <c r="E14" s="2">
-        <v>84.0</v>
+        <v>80.0</v>
       </c>
       <c r="F14" s="2">
         <v>0.0</v>
@@ -902,10 +929,10 @@
         <v>8.0</v>
       </c>
       <c r="H14" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I14" s="2">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="J14" s="2">
         <v>2.0</v>
@@ -922,13 +949,13 @@
         <v>25.3</v>
       </c>
       <c r="C15" s="2">
-        <v>33.0</v>
+        <v>33.5</v>
       </c>
       <c r="D15" s="2">
-        <v>28.4</v>
+        <v>28.6</v>
       </c>
       <c r="E15" s="2">
-        <v>87.0</v>
+        <v>83.0</v>
       </c>
       <c r="F15" s="2">
         <v>0.0</v>
@@ -937,51 +964,51 @@
         <v>8.0</v>
       </c>
       <c r="H15" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I15" s="2">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="J15" s="2">
         <v>2.0</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2">
-        <v>25.6</v>
+        <v>25.3</v>
       </c>
       <c r="C16" s="2">
-        <v>31.7</v>
+        <v>32.8</v>
       </c>
       <c r="D16" s="2">
-        <v>27.7</v>
+        <v>27.8</v>
       </c>
       <c r="E16" s="2">
-        <v>88.0</v>
+        <v>86.0</v>
       </c>
       <c r="F16" s="2">
         <v>0.0</v>
       </c>
       <c r="G16" s="2">
-        <v>7.0</v>
+        <v>6.5</v>
       </c>
       <c r="H16" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I16" s="2">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="J16" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -989,34 +1016,34 @@
         <v>33</v>
       </c>
       <c r="B17" s="2">
-        <v>23.6</v>
+        <v>23.8</v>
       </c>
       <c r="C17" s="2">
-        <v>30.9</v>
+        <v>31.8</v>
       </c>
       <c r="D17" s="2">
-        <v>26.9</v>
+        <v>27.4</v>
       </c>
       <c r="E17" s="2">
-        <v>86.0</v>
+        <v>81.0</v>
       </c>
       <c r="F17" s="2">
-        <v>33.4</v>
+        <v>30.2</v>
       </c>
       <c r="G17" s="2">
-        <v>7.7</v>
+        <v>6.9</v>
       </c>
       <c r="H17" s="2">
         <v>3.0</v>
       </c>
       <c r="I17" s="2">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="J17" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1024,34 +1051,34 @@
         <v>34</v>
       </c>
       <c r="B18" s="2">
-        <v>25.0</v>
+        <v>23.9</v>
       </c>
       <c r="C18" s="2">
-        <v>31.8</v>
+        <v>32.5</v>
       </c>
       <c r="D18" s="2">
-        <v>27.7</v>
+        <v>27.9</v>
       </c>
       <c r="E18" s="2">
-        <v>84.0</v>
+        <v>79.0</v>
       </c>
       <c r="F18" s="2">
-        <v>1.1</v>
+        <v>0.2</v>
       </c>
       <c r="G18" s="2">
-        <v>4.7</v>
+        <v>4.0</v>
       </c>
       <c r="H18" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I18" s="2">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="J18" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1059,28 +1086,28 @@
         <v>35</v>
       </c>
       <c r="B19" s="2">
-        <v>25.0</v>
+        <v>24.6</v>
       </c>
       <c r="C19" s="2">
-        <v>31.2</v>
+        <v>31.8</v>
       </c>
       <c r="D19" s="2">
         <v>27.3</v>
       </c>
       <c r="E19" s="2">
-        <v>86.0</v>
+        <v>83.0</v>
       </c>
       <c r="F19" s="2">
-        <v>12.7</v>
+        <v>13.2</v>
       </c>
       <c r="G19" s="2">
         <v>8.0</v>
       </c>
       <c r="H19" s="2">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="I19" s="2">
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="J19" s="2">
         <v>3.0</v>
@@ -1094,34 +1121,34 @@
         <v>36</v>
       </c>
       <c r="B20" s="2">
-        <v>25.2</v>
+        <v>25.3</v>
       </c>
       <c r="C20" s="2">
-        <v>32.0</v>
+        <v>32.6</v>
       </c>
       <c r="D20" s="2">
-        <v>28.0</v>
+        <v>28.4</v>
       </c>
       <c r="E20" s="2">
-        <v>81.0</v>
+        <v>74.0</v>
       </c>
       <c r="F20" s="2">
         <v>0.0</v>
       </c>
       <c r="G20" s="2">
-        <v>7.1</v>
+        <v>6.6</v>
       </c>
       <c r="H20" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I20" s="2">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="J20" s="2">
         <v>2.0</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1129,25 +1156,25 @@
         <v>37</v>
       </c>
       <c r="B21" s="2">
-        <v>25.5</v>
+        <v>25.2</v>
       </c>
       <c r="C21" s="2">
-        <v>31.9</v>
+        <v>32.4</v>
       </c>
       <c r="D21" s="2">
-        <v>28.0</v>
+        <v>28.1</v>
       </c>
       <c r="E21" s="2">
-        <v>87.0</v>
+        <v>84.0</v>
       </c>
       <c r="F21" s="2">
-        <v>3.0</v>
+        <v>5.2</v>
       </c>
       <c r="G21" s="2">
-        <v>6.3</v>
+        <v>7.0</v>
       </c>
       <c r="H21" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I21" s="2">
         <v>280</v>
@@ -1164,34 +1191,34 @@
         <v>38</v>
       </c>
       <c r="B22" s="2">
-        <v>25.2</v>
+        <v>24.9</v>
       </c>
       <c r="C22" s="2">
-        <v>31.7</v>
+        <v>32.3</v>
       </c>
       <c r="D22" s="2">
-        <v>28.0</v>
+        <v>28.2</v>
       </c>
       <c r="E22" s="2">
-        <v>88.0</v>
+        <v>86.0</v>
       </c>
       <c r="F22" s="2">
-        <v>26.8</v>
+        <v>19.6</v>
       </c>
       <c r="G22" s="2">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
       <c r="H22" s="2">
         <v>5.0</v>
       </c>
       <c r="I22" s="2">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="J22" s="2">
         <v>2.0</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1199,31 +1226,31 @@
         <v>39</v>
       </c>
       <c r="B23" s="2">
-        <v>24.8</v>
+        <v>24.5</v>
       </c>
       <c r="C23" s="2">
-        <v>32.2</v>
+        <v>33.6</v>
       </c>
       <c r="D23" s="2">
-        <v>28.0</v>
+        <v>28.2</v>
       </c>
       <c r="E23" s="2">
-        <v>83.0</v>
+        <v>79.0</v>
       </c>
       <c r="F23" s="2">
-        <v>3.1</v>
+        <v>1.4</v>
       </c>
       <c r="G23" s="2">
-        <v>8.0</v>
+        <v>7.5</v>
       </c>
       <c r="H23" s="2">
         <v>5.0</v>
       </c>
       <c r="I23" s="2">
-        <v>290</v>
+        <v>310</v>
       </c>
       <c r="J23" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>24</v>
@@ -1234,31 +1261,31 @@
         <v>40</v>
       </c>
       <c r="B24" s="2">
-        <v>25.0</v>
+        <v>24.7</v>
       </c>
       <c r="C24" s="2">
-        <v>32.4</v>
+        <v>33.5</v>
       </c>
       <c r="D24" s="2">
-        <v>28.4</v>
+        <v>28.6</v>
       </c>
       <c r="E24" s="2">
-        <v>79.0</v>
+        <v>74.0</v>
       </c>
       <c r="F24" s="2">
         <v>0.0</v>
       </c>
       <c r="G24" s="2">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
       <c r="H24" s="2">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="I24" s="2">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="J24" s="2">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>24</v>
@@ -1269,34 +1296,34 @@
         <v>41</v>
       </c>
       <c r="B25" s="2">
-        <v>25.3</v>
+        <v>25.2</v>
       </c>
       <c r="C25" s="2">
-        <v>32.4</v>
+        <v>33.0</v>
       </c>
       <c r="D25" s="2">
-        <v>28.3</v>
+        <v>28.5</v>
       </c>
       <c r="E25" s="2">
-        <v>78.0</v>
+        <v>72.0</v>
       </c>
       <c r="F25" s="2">
         <v>0.0</v>
       </c>
       <c r="G25" s="2">
-        <v>6.4</v>
+        <v>3.6</v>
       </c>
       <c r="H25" s="2">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="I25" s="2">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="J25" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1304,16 +1331,16 @@
         <v>42</v>
       </c>
       <c r="B26" s="2">
-        <v>24.9</v>
+        <v>25.4</v>
       </c>
       <c r="C26" s="2">
-        <v>32.0</v>
+        <v>32.8</v>
       </c>
       <c r="D26" s="2">
-        <v>28.4</v>
+        <v>28.5</v>
       </c>
       <c r="E26" s="2">
-        <v>84.0</v>
+        <v>80.0</v>
       </c>
       <c r="F26" s="2">
         <v>0.0</v>
@@ -1322,16 +1349,16 @@
         <v>8.0</v>
       </c>
       <c r="H26" s="2">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="I26" s="2">
         <v>280</v>
       </c>
       <c r="J26" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1339,16 +1366,16 @@
         <v>43</v>
       </c>
       <c r="B27" s="2">
-        <v>26.0</v>
+        <v>25.7</v>
       </c>
       <c r="C27" s="2">
-        <v>32.4</v>
+        <v>33.5</v>
       </c>
       <c r="D27" s="2">
-        <v>28.4</v>
+        <v>28.6</v>
       </c>
       <c r="E27" s="2">
-        <v>86.0</v>
+        <v>79.0</v>
       </c>
       <c r="F27" s="2">
         <v>0.0</v>
@@ -1360,13 +1387,13 @@
         <v>3.0</v>
       </c>
       <c r="I27" s="2">
-        <v>290</v>
+        <v>250</v>
       </c>
       <c r="J27" s="2">
         <v>1.0</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1374,16 +1401,16 @@
         <v>44</v>
       </c>
       <c r="B28" s="2">
-        <v>25.0</v>
+        <v>24.8</v>
       </c>
       <c r="C28" s="2">
-        <v>33.8</v>
+        <v>33.6</v>
       </c>
       <c r="D28" s="2">
-        <v>28.5</v>
+        <v>28.3</v>
       </c>
       <c r="E28" s="2">
-        <v>81.0</v>
+        <v>78.0</v>
       </c>
       <c r="F28" s="2">
         <v>0.0</v>
@@ -1392,13 +1419,13 @@
         <v>2.7</v>
       </c>
       <c r="H28" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I28" s="2">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="J28" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>29</v>
@@ -1409,16 +1436,16 @@
         <v>45</v>
       </c>
       <c r="B29" s="2">
-        <v>23.9</v>
+        <v>23.8</v>
       </c>
       <c r="C29" s="2">
-        <v>31.9</v>
+        <v>33.0</v>
       </c>
       <c r="D29" s="2">
         <v>28.0</v>
       </c>
       <c r="E29" s="2">
-        <v>83.0</v>
+        <v>79.0</v>
       </c>
       <c r="F29" s="2">
         <v>0.0</v>
@@ -1427,10 +1454,10 @@
         <v>7.6</v>
       </c>
       <c r="H29" s="2">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="I29" s="2">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="J29" s="2">
         <v>2.0</v>
@@ -1444,16 +1471,16 @@
         <v>46</v>
       </c>
       <c r="B30" s="2">
-        <v>26.0</v>
+        <v>24.4</v>
       </c>
       <c r="C30" s="2">
-        <v>30.4</v>
+        <v>31.0</v>
       </c>
       <c r="D30" s="2">
-        <v>27.0</v>
+        <v>27.3</v>
       </c>
       <c r="E30" s="2">
-        <v>90.0</v>
+        <v>85.0</v>
       </c>
       <c r="F30" s="2">
         <v>8888.0</v>
@@ -1462,39 +1489,39 @@
         <v>8.0</v>
       </c>
       <c r="H30" s="2">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I30" s="2">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="J30" s="2">
         <v>3.0</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2">
-        <v>23.6</v>
+        <v>23.2</v>
       </c>
       <c r="C31" s="2">
-        <v>31.0</v>
+        <v>31.4</v>
       </c>
       <c r="D31" s="2">
-        <v>26.8</v>
+        <v>26.9</v>
       </c>
       <c r="E31" s="2">
-        <v>82.0</v>
+        <v>77.0</v>
       </c>
       <c r="F31" s="2">
-        <v>58.8</v>
+        <v>48.0</v>
       </c>
       <c r="G31" s="2">
-        <v>2.5</v>
+        <v>1.6</v>
       </c>
       <c r="H31" s="2">
         <v>4.0</v>
@@ -1511,31 +1538,31 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" s="2">
-        <v>23.8</v>
+        <v>23.9</v>
       </c>
       <c r="C32" s="2">
-        <v>31.6</v>
+        <v>32.6</v>
       </c>
       <c r="D32" s="2">
-        <v>27.4</v>
+        <v>27.6</v>
       </c>
       <c r="E32" s="2">
-        <v>85.0</v>
+        <v>81.0</v>
       </c>
       <c r="F32" s="2">
-        <v>8888.0</v>
+        <v>0.0</v>
       </c>
       <c r="G32" s="2">
-        <v>3.3</v>
+        <v>2.6</v>
       </c>
       <c r="H32" s="2">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="I32" s="2">
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="J32" s="2">
         <v>2.0</v>
@@ -1545,81 +1572,326 @@
       </c>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
+      <c r="A33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="2">
+        <v>24.9</v>
+      </c>
+      <c r="C33" s="2">
+        <v>32.1</v>
+      </c>
+      <c r="D33" s="2">
+        <v>28.1</v>
+      </c>
+      <c r="E33" s="2">
+        <v>86.0</v>
+      </c>
+      <c r="F33" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="G33" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="H33" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="I33" s="2">
+        <v>310</v>
+      </c>
+      <c r="J33" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="2">
+        <v>25.3</v>
+      </c>
+      <c r="C34" s="2">
+        <v>32.2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>28.5</v>
+      </c>
+      <c r="E34" s="2">
+        <v>72.0</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G34" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="H34" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="I34" s="2">
+        <v>280</v>
+      </c>
+      <c r="J34" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="2">
+        <v>25.4</v>
+      </c>
+      <c r="C35" s="2">
+        <v>32.9</v>
+      </c>
+      <c r="D35" s="2">
+        <v>29.0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>71.0</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="H35" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="I35" s="2">
+        <v>270</v>
+      </c>
+      <c r="J35" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" t="s">
-        <v>49</v>
+      <c r="A36" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="2">
+        <v>24.9</v>
+      </c>
+      <c r="C36" s="2">
+        <v>32.7</v>
+      </c>
+      <c r="D36" s="2">
+        <v>28.5</v>
+      </c>
+      <c r="E36" s="2">
+        <v>80.0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G36" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="H36" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="I36" s="2">
+        <v>250</v>
+      </c>
+      <c r="J36" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" t="s">
-        <v>50</v>
+      <c r="A37" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="2">
+        <v>25.4</v>
+      </c>
+      <c r="C37" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="D37" s="2">
+        <v>28.8</v>
+      </c>
+      <c r="E37" s="2">
+        <v>80.0</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="I37" s="2">
+        <v>250</v>
+      </c>
+      <c r="J37" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" t="s">
-        <v>51</v>
+      <c r="A38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="2">
+        <v>25.6</v>
+      </c>
+      <c r="C38" s="2">
+        <v>33.7</v>
+      </c>
+      <c r="D38" s="2">
+        <v>28.8</v>
+      </c>
+      <c r="E38" s="2">
+        <v>81.0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="I38" s="2">
+        <v>180</v>
+      </c>
+      <c r="J38" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" t="s">
-        <v>52</v>
+      <c r="A39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="2">
+        <v>25.6</v>
+      </c>
+      <c r="C39" s="2">
+        <v>33.2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>28.7</v>
+      </c>
+      <c r="E39" s="2">
+        <v>79.0</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="H39" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="I39" s="2">
+        <v>240</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" t="s">
-        <v>55</v>
-      </c>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>